<commit_message>
HKD New framework (work in progress)
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD/HKD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD/HKD_YCSTDBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19125" windowHeight="12255" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19125" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
@@ -1462,8 +1462,8 @@
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
-        <row r="15">
-          <cell r="K15" t="str">
+        <row r="13">
+          <cell r="D13" t="str">
             <v>HKDSTD#0000</v>
           </cell>
         </row>
@@ -1772,7 +1772,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1792,7 +1792,7 @@
     <row r="1" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="77" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.6.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - Jul 20 2015 13:11:27</v>
+        <v>QuantLibXL 1.7.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - Sep 24 2015 15:39:48</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D14" s="102" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,_xll.ohPack(Selected!D2:D126),,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>HKDYCSTD#0005</v>
+        <v>HKDYCSTD#0001</v>
       </c>
       <c r="E14" s="80"/>
       <c r="F14" s="122"/>
@@ -2154,7 +2154,7 @@
     <row r="26" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="78"/>
       <c r="C26" s="116" t="str">
-        <f>[1]Hibor!$K$15</f>
+        <f>[1]Hibor!$D$13</f>
         <v>HKDSTD#0000</v>
       </c>
       <c r="D26" s="90" t="b">
@@ -2217,7 +2217,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I2" sqref="I2:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2263,7 +2263,7 @@
     <row r="2" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="str">
         <f>Deposits!E3</f>
-        <v>obj_00138#0005</v>
+        <v>obj_00133#0001</v>
       </c>
       <c r="B2" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A2)</f>
@@ -2288,14 +2288,14 @@
         <v>42180</v>
       </c>
       <c r="I2" s="12">
-        <f>_xll.qlRateHelperLatestDate($A2,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A2,Trigger)</f>
         <v>42181</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="str">
         <f>Deposits!E4</f>
-        <v>obj_0013f#0003</v>
+        <v>obj_00135#0001</v>
       </c>
       <c r="B3" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A3)</f>
@@ -2320,14 +2320,14 @@
         <v>42180</v>
       </c>
       <c r="I3" s="12">
-        <f>_xll.qlRateHelperLatestDate($A3,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A3,Trigger)</f>
         <v>42187</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="str">
         <f>Deposits!E5</f>
-        <v>obj_0013e#0003</v>
+        <v>obj_00138#0001</v>
       </c>
       <c r="B4" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A4)</f>
@@ -2352,14 +2352,14 @@
         <v>42180</v>
       </c>
       <c r="I4" s="12">
-        <f>_xll.qlRateHelperLatestDate($A4,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A4,Trigger)</f>
         <v>42194</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="str">
         <f>Deposits!E6</f>
-        <v>obj_00139#0003</v>
+        <v>obj_00139#0001</v>
       </c>
       <c r="B5" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A5)</f>
@@ -2384,14 +2384,14 @@
         <v>42180</v>
       </c>
       <c r="I5" s="12">
-        <f>_xll.qlRateHelperLatestDate($A5,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A5,Trigger)</f>
         <v>42212</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="str">
         <f>Deposits!E7</f>
-        <v>obj_0013d#0003</v>
+        <v>obj_00136#0001</v>
       </c>
       <c r="B6" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A6)</f>
@@ -2416,14 +2416,14 @@
         <v>42180</v>
       </c>
       <c r="I6" s="12">
-        <f>_xll.qlRateHelperLatestDate($A6,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A6,Trigger)</f>
         <v>42241</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="str">
         <f>Deposits!E8</f>
-        <v>obj_0013a#0003</v>
+        <v>obj_0013b#0001</v>
       </c>
       <c r="B7" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A7)</f>
@@ -2448,14 +2448,14 @@
         <v>42180</v>
       </c>
       <c r="I7" s="12">
-        <f>_xll.qlRateHelperLatestDate($A7,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A7,Trigger)</f>
         <v>42272</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="str">
         <f>Deposits!E9</f>
-        <v>obj_00140#0003</v>
+        <v>obj_0013a#0001</v>
       </c>
       <c r="B8" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A8)</f>
@@ -2480,14 +2480,14 @@
         <v>42180</v>
       </c>
       <c r="I8" s="12">
-        <f>_xll.qlRateHelperLatestDate($A8,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A8,Trigger)</f>
         <v>42366</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="str">
         <f>Deposits!E10</f>
-        <v>obj_0013c#0003</v>
+        <v>obj_00134#0001</v>
       </c>
       <c r="B9" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A9)</f>
@@ -2512,14 +2512,14 @@
         <v>42180</v>
       </c>
       <c r="I9" s="12">
-        <f>_xll.qlRateHelperLatestDate($A9,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A9,Trigger)</f>
         <v>42458</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="str">
         <f>Deposits!E11</f>
-        <v>obj_0013b#0003</v>
+        <v>obj_00137#0001</v>
       </c>
       <c r="B10" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(A10)</f>
@@ -2544,14 +2544,14 @@
         <v>42180</v>
       </c>
       <c r="I10" s="14">
-        <f>_xll.qlRateHelperLatestDate($A10,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A10,Trigger)</f>
         <v>42548</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="str">
         <f>Swaps!L6</f>
-        <v>obj_00127#0001</v>
+        <v>obj_00124#0001</v>
       </c>
       <c r="B11" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A11)</f>
@@ -2580,14 +2580,14 @@
         <v>42181</v>
       </c>
       <c r="I11" s="12">
-        <f>_xll.qlRateHelperLatestDate($A11,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A11,Trigger)</f>
         <v>42548</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="str">
         <f>Swaps!L7</f>
-        <v>obj_00130#0001</v>
+        <v>obj_00122#0001</v>
       </c>
       <c r="B12" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A12)</f>
@@ -2616,14 +2616,14 @@
         <v>42181</v>
       </c>
       <c r="I12" s="12">
-        <f>_xll.qlRateHelperLatestDate($A12,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A12,Trigger)</f>
         <v>42639</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="str">
         <f>Swaps!L8</f>
-        <v>obj_00128#0001</v>
+        <v>obj_00125#0001</v>
       </c>
       <c r="B13" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A13)</f>
@@ -2652,7 +2652,7 @@
         <v>42181</v>
       </c>
       <c r="I13" s="12">
-        <f>_xll.qlRateHelperLatestDate($A13,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A13,Trigger)</f>
         <v>42731</v>
       </c>
     </row>
@@ -2688,14 +2688,14 @@
         <v>42181</v>
       </c>
       <c r="I14" s="12">
-        <f>_xll.qlRateHelperLatestDate($A14,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A14,Trigger)</f>
         <v>42821</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="str">
         <f>Swaps!L10</f>
-        <v>obj_00136#0001</v>
+        <v>obj_00131#0001</v>
       </c>
       <c r="B15" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A15)</f>
@@ -2724,14 +2724,14 @@
         <v>42181</v>
       </c>
       <c r="I15" s="12">
-        <f>_xll.qlRateHelperLatestDate($A15,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A15,Trigger)</f>
         <v>42912</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="str">
         <f>Swaps!L11</f>
-        <v>obj_00134#0001</v>
+        <v>obj_00129#0001</v>
       </c>
       <c r="B16" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A16)</f>
@@ -2760,14 +2760,14 @@
         <v>42181</v>
       </c>
       <c r="I16" s="12">
-        <f>_xll.qlRateHelperLatestDate($A16,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A16,Trigger)</f>
         <v>43277</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="str">
         <f>Swaps!L12</f>
-        <v>obj_00131#0001</v>
+        <v>obj_0012e#0001</v>
       </c>
       <c r="B17" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A17)</f>
@@ -2796,14 +2796,14 @@
         <v>42181</v>
       </c>
       <c r="I17" s="12">
-        <f>_xll.qlRateHelperLatestDate($A17,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A17,Trigger)</f>
         <v>43642</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="str">
         <f>Swaps!L13</f>
-        <v>obj_00123#0001</v>
+        <v>obj_00127#0001</v>
       </c>
       <c r="B18" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A18)</f>
@@ -2832,14 +2832,14 @@
         <v>42181</v>
       </c>
       <c r="I18" s="12">
-        <f>_xll.qlRateHelperLatestDate($A18,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A18,Trigger)</f>
         <v>44008</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="str">
         <f>Swaps!L14</f>
-        <v>obj_00125#0001</v>
+        <v>obj_0011f#0001</v>
       </c>
       <c r="B19" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A19)</f>
@@ -2868,14 +2868,14 @@
         <v>42181</v>
       </c>
       <c r="I19" s="12">
-        <f>_xll.qlRateHelperLatestDate($A19,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A19,Trigger)</f>
         <v>44375</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="str">
         <f>Swaps!L15</f>
-        <v>obj_00137#0001</v>
+        <v>obj_00132#0001</v>
       </c>
       <c r="B20" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A20)</f>
@@ -2904,14 +2904,14 @@
         <v>42181</v>
       </c>
       <c r="I20" s="12">
-        <f>_xll.qlRateHelperLatestDate($A20,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A20,Trigger)</f>
         <v>44739</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="str">
         <f>Swaps!L16</f>
-        <v>obj_0012a#0001</v>
+        <v>obj_00128#0001</v>
       </c>
       <c r="B21" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A21)</f>
@@ -2940,14 +2940,14 @@
         <v>42181</v>
       </c>
       <c r="I21" s="12">
-        <f>_xll.qlRateHelperLatestDate($A21,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A21,Trigger)</f>
         <v>45103</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="str">
         <f>Swaps!L17</f>
-        <v>obj_0012d#0001</v>
+        <v>obj_00121#0001</v>
       </c>
       <c r="B22" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A22)</f>
@@ -2976,14 +2976,14 @@
         <v>42181</v>
       </c>
       <c r="I22" s="12">
-        <f>_xll.qlRateHelperLatestDate($A22,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A22,Trigger)</f>
         <v>45469</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="str">
         <f>Swaps!L18</f>
-        <v>obj_00122#0001</v>
+        <v>obj_0011d#0001</v>
       </c>
       <c r="B23" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A23)</f>
@@ -3012,14 +3012,14 @@
         <v>42181</v>
       </c>
       <c r="I23" s="12">
-        <f>_xll.qlRateHelperLatestDate($A23,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A23,Trigger)</f>
         <v>45834</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="str">
         <f>Swaps!L19</f>
-        <v>obj_00133#0001</v>
+        <v>obj_0012b#0001</v>
       </c>
       <c r="B24" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A24)</f>
@@ -3048,14 +3048,14 @@
         <v>42181</v>
       </c>
       <c r="I24" s="12">
-        <f>_xll.qlRateHelperLatestDate($A24,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A24,Trigger)</f>
         <v>46199</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="str">
         <f>Swaps!L20</f>
-        <v>obj_0012e#0001</v>
+        <v>obj_00123#0001</v>
       </c>
       <c r="B25" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A25)</f>
@@ -3084,14 +3084,14 @@
         <v>42181</v>
       </c>
       <c r="I25" s="12">
-        <f>_xll.qlRateHelperLatestDate($A25,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A25,Trigger)</f>
         <v>46566</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="str">
         <f>Swaps!L21</f>
-        <v>obj_00124#0001</v>
+        <v>obj_0012a#0001</v>
       </c>
       <c r="B26" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A26)</f>
@@ -3120,14 +3120,14 @@
         <v>42181</v>
       </c>
       <c r="I26" s="12">
-        <f>_xll.qlRateHelperLatestDate($A26,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A26,Trigger)</f>
         <v>46930</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="str">
         <f>Swaps!L22</f>
-        <v>obj_0012f#0001</v>
+        <v>obj_0012d#0001</v>
       </c>
       <c r="B27" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A27)</f>
@@ -3156,14 +3156,14 @@
         <v>42181</v>
       </c>
       <c r="I27" s="12">
-        <f>_xll.qlRateHelperLatestDate($A27,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A27,Trigger)</f>
         <v>47295</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="str">
         <f>Swaps!L23</f>
-        <v>obj_00121#0001</v>
+        <v>obj_0011c#0001</v>
       </c>
       <c r="B28" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A28)</f>
@@ -3192,14 +3192,14 @@
         <v>42181</v>
       </c>
       <c r="I28" s="12">
-        <f>_xll.qlRateHelperLatestDate($A28,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A28,Trigger)</f>
         <v>47660</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="str">
         <f>Swaps!L24</f>
-        <v>obj_0012b#0001</v>
+        <v>obj_0011e#0001</v>
       </c>
       <c r="B29" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A29)</f>
@@ -3228,14 +3228,14 @@
         <v>42181</v>
       </c>
       <c r="I29" s="12">
-        <f>_xll.qlRateHelperLatestDate($A29,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A29,Trigger)</f>
         <v>48025</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="str">
         <f>Swaps!L25</f>
-        <v>obj_00126#0001</v>
+        <v>obj_0012f#0001</v>
       </c>
       <c r="B30" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A30)</f>
@@ -3264,14 +3264,14 @@
         <v>42181</v>
       </c>
       <c r="I30" s="12">
-        <f>_xll.qlRateHelperLatestDate($A30,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A30,Trigger)</f>
         <v>48393</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="str">
         <f>Swaps!L26</f>
-        <v>obj_00129#0001</v>
+        <v>obj_00126#0001</v>
       </c>
       <c r="B31" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A31)</f>
@@ -3300,14 +3300,14 @@
         <v>42181</v>
       </c>
       <c r="I31" s="12">
-        <f>_xll.qlRateHelperLatestDate($A31,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A31,Trigger)</f>
         <v>48757</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="str">
         <f>Swaps!L27</f>
-        <v>obj_00132#0001</v>
+        <v>obj_00120#0001</v>
       </c>
       <c r="B32" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A32)</f>
@@ -3336,14 +3336,14 @@
         <v>42181</v>
       </c>
       <c r="I32" s="12">
-        <f>_xll.qlRateHelperLatestDate($A32,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A32,Trigger)</f>
         <v>49121</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="str">
         <f>Swaps!L28</f>
-        <v>obj_00135#0001</v>
+        <v>obj_00130#0001</v>
       </c>
       <c r="B33" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A33)</f>
@@ -3372,7 +3372,7 @@
         <v>42181</v>
       </c>
       <c r="I33" s="12">
-        <f>_xll.qlRateHelperLatestDate($A33,Trigger)</f>
+        <f>_xll.qlRateHelperPillarDate($A33,Trigger)</f>
         <v>49486</v>
       </c>
     </row>
@@ -3401,8 +3401,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3454,7 +3454,7 @@
       </c>
       <c r="D2" s="21" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_00140</v>
+        <v>obj_0013a</v>
       </c>
       <c r="E2" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D2)</f>
@@ -3473,7 +3473,7 @@
         <v>42180</v>
       </c>
       <c r="I2" s="28">
-        <f>_xll.qlRateHelperLatestDate($D2)</f>
+        <f>_xll.qlRateHelperPillarDate($D2)</f>
         <v>42366</v>
       </c>
       <c r="J2" s="18">
@@ -3489,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="21" t="str">
-        <v>obj_00127</v>
+        <v>obj_00124</v>
       </c>
       <c r="E3" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D3)</f>
@@ -3508,7 +3508,7 @@
         <v>42181</v>
       </c>
       <c r="I3" s="28">
-        <f>_xll.qlRateHelperLatestDate($D3)</f>
+        <f>_xll.qlRateHelperPillarDate($D3)</f>
         <v>42548</v>
       </c>
       <c r="J3" s="18">
@@ -3524,7 +3524,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="21" t="str">
-        <v>obj_00128</v>
+        <v>obj_00125</v>
       </c>
       <c r="E4" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D4)</f>
@@ -3543,7 +3543,7 @@
         <v>42181</v>
       </c>
       <c r="I4" s="28">
-        <f>_xll.qlRateHelperLatestDate($D4)</f>
+        <f>_xll.qlRateHelperPillarDate($D4)</f>
         <v>42731</v>
       </c>
       <c r="J4" s="18">
@@ -3559,7 +3559,7 @@
         <v>63</v>
       </c>
       <c r="D5" s="21" t="str">
-        <v>obj_00136</v>
+        <v>obj_00131</v>
       </c>
       <c r="E5" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D5)</f>
@@ -3578,7 +3578,7 @@
         <v>42181</v>
       </c>
       <c r="I5" s="28">
-        <f>_xll.qlRateHelperLatestDate($D5)</f>
+        <f>_xll.qlRateHelperPillarDate($D5)</f>
         <v>42912</v>
       </c>
       <c r="J5" s="18">
@@ -3590,7 +3590,7 @@
       <c r="A6" s="54"/>
       <c r="B6" s="54"/>
       <c r="D6" s="21" t="str">
-        <v>obj_00134</v>
+        <v>obj_00129</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D6)</f>
@@ -3609,7 +3609,7 @@
         <v>42181</v>
       </c>
       <c r="I6" s="28">
-        <f>_xll.qlRateHelperLatestDate($D6)</f>
+        <f>_xll.qlRateHelperPillarDate($D6)</f>
         <v>43277</v>
       </c>
       <c r="J6" s="18">
@@ -3619,7 +3619,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" s="21" t="str">
-        <v>obj_00131</v>
+        <v>obj_0012e</v>
       </c>
       <c r="E7" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D7)</f>
@@ -3638,7 +3638,7 @@
         <v>42181</v>
       </c>
       <c r="I7" s="28">
-        <f>_xll.qlRateHelperLatestDate($D7)</f>
+        <f>_xll.qlRateHelperPillarDate($D7)</f>
         <v>43642</v>
       </c>
       <c r="J7" s="18">
@@ -3648,7 +3648,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="21" t="str">
-        <v>obj_00123</v>
+        <v>obj_00127</v>
       </c>
       <c r="E8" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D8)</f>
@@ -3667,7 +3667,7 @@
         <v>42181</v>
       </c>
       <c r="I8" s="28">
-        <f>_xll.qlRateHelperLatestDate($D8)</f>
+        <f>_xll.qlRateHelperPillarDate($D8)</f>
         <v>44008</v>
       </c>
       <c r="J8" s="18">
@@ -3677,7 +3677,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D9" s="21" t="str">
-        <v>obj_00137</v>
+        <v>obj_00132</v>
       </c>
       <c r="E9" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D9)</f>
@@ -3696,7 +3696,7 @@
         <v>42181</v>
       </c>
       <c r="I9" s="28">
-        <f>_xll.qlRateHelperLatestDate($D9)</f>
+        <f>_xll.qlRateHelperPillarDate($D9)</f>
         <v>44739</v>
       </c>
       <c r="J9" s="18">
@@ -3706,7 +3706,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D10" s="21" t="str">
-        <v>obj_00122</v>
+        <v>obj_0011d</v>
       </c>
       <c r="E10" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D10)</f>
@@ -3725,7 +3725,7 @@
         <v>42181</v>
       </c>
       <c r="I10" s="28">
-        <f>_xll.qlRateHelperLatestDate($D10)</f>
+        <f>_xll.qlRateHelperPillarDate($D10)</f>
         <v>45834</v>
       </c>
       <c r="J10" s="18">
@@ -3735,7 +3735,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="21" t="str">
-        <v>obj_0012e</v>
+        <v>obj_00123</v>
       </c>
       <c r="E11" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D11)</f>
@@ -3754,7 +3754,7 @@
         <v>42181</v>
       </c>
       <c r="I11" s="28">
-        <f>_xll.qlRateHelperLatestDate($D11)</f>
+        <f>_xll.qlRateHelperPillarDate($D11)</f>
         <v>46566</v>
       </c>
       <c r="J11" s="18">
@@ -3764,7 +3764,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="21" t="str">
-        <v>obj_00121</v>
+        <v>obj_0011c</v>
       </c>
       <c r="E12" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D12)</f>
@@ -3783,7 +3783,7 @@
         <v>42181</v>
       </c>
       <c r="I12" s="28">
-        <f>_xll.qlRateHelperLatestDate($D12)</f>
+        <f>_xll.qlRateHelperPillarDate($D12)</f>
         <v>47660</v>
       </c>
       <c r="J12" s="18">
@@ -3793,7 +3793,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="21" t="str">
-        <v>obj_00135</v>
+        <v>obj_00130</v>
       </c>
       <c r="E13" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D13)</f>
@@ -3812,7 +3812,7 @@
         <v>42181</v>
       </c>
       <c r="I13" s="28">
-        <f>_xll.qlRateHelperLatestDate($D13)</f>
+        <f>_xll.qlRateHelperPillarDate($D13)</f>
         <v>49486</v>
       </c>
       <c r="J13" s="18">
@@ -3841,7 +3841,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I14" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D14)</f>
+        <f>_xll.qlRateHelperPillarDate($D14)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J14" s="18" t="e">
@@ -3869,7 +3869,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I15" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D15)</f>
+        <f>_xll.qlRateHelperPillarDate($D15)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J15" s="18" t="e">
@@ -3897,7 +3897,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I16" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D16)</f>
+        <f>_xll.qlRateHelperPillarDate($D16)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J16" s="18" t="e">
@@ -3925,7 +3925,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I17" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D17)</f>
+        <f>_xll.qlRateHelperPillarDate($D17)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J17" s="18" t="e">
@@ -3953,7 +3953,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I18" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D18)</f>
+        <f>_xll.qlRateHelperPillarDate($D18)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J18" s="18" t="e">
@@ -3981,7 +3981,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I19" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D19)</f>
+        <f>_xll.qlRateHelperPillarDate($D19)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J19" s="18" t="e">
@@ -4009,7 +4009,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I20" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D20)</f>
+        <f>_xll.qlRateHelperPillarDate($D20)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J20" s="18" t="e">
@@ -4037,7 +4037,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I21" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D21)</f>
+        <f>_xll.qlRateHelperPillarDate($D21)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J21" s="18" t="e">
@@ -4065,7 +4065,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I22" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D22)</f>
+        <f>_xll.qlRateHelperPillarDate($D22)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J22" s="18" t="e">
@@ -4093,7 +4093,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I23" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D23)</f>
+        <f>_xll.qlRateHelperPillarDate($D23)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J23" s="18" t="e">
@@ -4121,7 +4121,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I24" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D24)</f>
+        <f>_xll.qlRateHelperPillarDate($D24)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J24" s="18" t="e">
@@ -4149,7 +4149,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I25" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D25)</f>
+        <f>_xll.qlRateHelperPillarDate($D25)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J25" s="18" t="e">
@@ -4177,7 +4177,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I26" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D26)</f>
+        <f>_xll.qlRateHelperPillarDate($D26)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J26" s="18" t="e">
@@ -4205,7 +4205,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I27" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D27)</f>
+        <f>_xll.qlRateHelperPillarDate($D27)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J27" s="18" t="e">
@@ -4233,7 +4233,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I28" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D28)</f>
+        <f>_xll.qlRateHelperPillarDate($D28)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J28" s="18" t="e">
@@ -4261,7 +4261,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I29" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D29)</f>
+        <f>_xll.qlRateHelperPillarDate($D29)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J29" s="18" t="e">
@@ -4289,7 +4289,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I30" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D30)</f>
+        <f>_xll.qlRateHelperPillarDate($D30)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J30" s="18" t="e">
@@ -4317,7 +4317,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I31" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D31)</f>
+        <f>_xll.qlRateHelperPillarDate($D31)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J31" s="18" t="e">
@@ -4345,7 +4345,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I32" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D32)</f>
+        <f>_xll.qlRateHelperPillarDate($D32)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J32" s="18" t="e">
@@ -4373,7 +4373,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I33" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D33)</f>
+        <f>_xll.qlRateHelperPillarDate($D33)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J33" s="18" t="e">
@@ -4401,7 +4401,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I34" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D34)</f>
+        <f>_xll.qlRateHelperPillarDate($D34)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J34" s="18" t="e">
@@ -4429,7 +4429,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I35" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D35)</f>
+        <f>_xll.qlRateHelperPillarDate($D35)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J35" s="18" t="e">
@@ -4457,7 +4457,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I36" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D36)</f>
+        <f>_xll.qlRateHelperPillarDate($D36)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J36" s="18" t="e">
@@ -4485,7 +4485,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I37" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D37)</f>
+        <f>_xll.qlRateHelperPillarDate($D37)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J37" s="18" t="e">
@@ -4513,7 +4513,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I38" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D38)</f>
+        <f>_xll.qlRateHelperPillarDate($D38)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J38" s="18" t="e">
@@ -4541,7 +4541,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I39" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D39)</f>
+        <f>_xll.qlRateHelperPillarDate($D39)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J39" s="18" t="e">
@@ -4569,7 +4569,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I40" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D40)</f>
+        <f>_xll.qlRateHelperPillarDate($D40)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J40" s="18" t="e">
@@ -4597,7 +4597,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I41" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D41)</f>
+        <f>_xll.qlRateHelperPillarDate($D41)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J41" s="18" t="e">
@@ -4625,7 +4625,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I42" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D42)</f>
+        <f>_xll.qlRateHelperPillarDate($D42)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J42" s="18" t="e">
@@ -4653,7 +4653,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I43" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D43)</f>
+        <f>_xll.qlRateHelperPillarDate($D43)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J43" s="18" t="e">
@@ -4681,7 +4681,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I44" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D44)</f>
+        <f>_xll.qlRateHelperPillarDate($D44)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J44" s="18" t="e">
@@ -4709,7 +4709,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I45" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D45)</f>
+        <f>_xll.qlRateHelperPillarDate($D45)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J45" s="18" t="e">
@@ -4737,7 +4737,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I46" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D46)</f>
+        <f>_xll.qlRateHelperPillarDate($D46)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J46" s="18" t="e">
@@ -4765,7 +4765,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I47" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D47)</f>
+        <f>_xll.qlRateHelperPillarDate($D47)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J47" s="18" t="e">
@@ -4793,7 +4793,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I48" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D48)</f>
+        <f>_xll.qlRateHelperPillarDate($D48)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J48" s="18" t="e">
@@ -4821,7 +4821,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I49" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D49)</f>
+        <f>_xll.qlRateHelperPillarDate($D49)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J49" s="18" t="e">
@@ -4849,7 +4849,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I50" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D50)</f>
+        <f>_xll.qlRateHelperPillarDate($D50)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J50" s="18" t="e">
@@ -4877,7 +4877,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I51" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D51)</f>
+        <f>_xll.qlRateHelperPillarDate($D51)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J51" s="18" t="e">
@@ -4905,7 +4905,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I52" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D52)</f>
+        <f>_xll.qlRateHelperPillarDate($D52)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J52" s="18" t="e">
@@ -4933,7 +4933,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I53" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D53)</f>
+        <f>_xll.qlRateHelperPillarDate($D53)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J53" s="18" t="e">
@@ -4961,7 +4961,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I54" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D54)</f>
+        <f>_xll.qlRateHelperPillarDate($D54)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J54" s="18" t="e">
@@ -4989,7 +4989,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I55" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D55)</f>
+        <f>_xll.qlRateHelperPillarDate($D55)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J55" s="18" t="e">
@@ -5017,7 +5017,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I56" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D56)</f>
+        <f>_xll.qlRateHelperPillarDate($D56)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J56" s="18" t="e">
@@ -5045,7 +5045,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I57" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D57)</f>
+        <f>_xll.qlRateHelperPillarDate($D57)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J57" s="18" t="e">
@@ -5073,7 +5073,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I58" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D58)</f>
+        <f>_xll.qlRateHelperPillarDate($D58)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J58" s="18" t="e">
@@ -5101,7 +5101,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I59" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D59)</f>
+        <f>_xll.qlRateHelperPillarDate($D59)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J59" s="18" t="e">
@@ -5129,7 +5129,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I60" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D60)</f>
+        <f>_xll.qlRateHelperPillarDate($D60)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J60" s="18" t="e">
@@ -5157,7 +5157,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I61" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D61)</f>
+        <f>_xll.qlRateHelperPillarDate($D61)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J61" s="18" t="e">
@@ -5185,7 +5185,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I62" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D62)</f>
+        <f>_xll.qlRateHelperPillarDate($D62)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J62" s="18" t="e">
@@ -5213,7 +5213,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I63" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D63)</f>
+        <f>_xll.qlRateHelperPillarDate($D63)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J63" s="18" t="e">
@@ -5241,7 +5241,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I64" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D64)</f>
+        <f>_xll.qlRateHelperPillarDate($D64)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J64" s="18" t="e">
@@ -5269,7 +5269,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I65" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D65)</f>
+        <f>_xll.qlRateHelperPillarDate($D65)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J65" s="18" t="e">
@@ -5297,7 +5297,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I66" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D66)</f>
+        <f>_xll.qlRateHelperPillarDate($D66)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J66" s="18" t="e">
@@ -5325,7 +5325,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I67" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D67)</f>
+        <f>_xll.qlRateHelperPillarDate($D67)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J67" s="18" t="e">
@@ -5353,7 +5353,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I68" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D68)</f>
+        <f>_xll.qlRateHelperPillarDate($D68)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J68" s="18" t="e">
@@ -5381,7 +5381,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I69" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D69)</f>
+        <f>_xll.qlRateHelperPillarDate($D69)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J69" s="18" t="e">
@@ -5409,7 +5409,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I70" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D70)</f>
+        <f>_xll.qlRateHelperPillarDate($D70)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J70" s="18" t="e">
@@ -5437,7 +5437,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I71" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D71)</f>
+        <f>_xll.qlRateHelperPillarDate($D71)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J71" s="18" t="e">
@@ -5465,7 +5465,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I72" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D72)</f>
+        <f>_xll.qlRateHelperPillarDate($D72)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J72" s="18" t="e">
@@ -5493,7 +5493,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I73" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D73)</f>
+        <f>_xll.qlRateHelperPillarDate($D73)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J73" s="18" t="e">
@@ -5521,7 +5521,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I74" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D74)</f>
+        <f>_xll.qlRateHelperPillarDate($D74)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J74" s="18" t="e">
@@ -5549,7 +5549,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I75" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D75)</f>
+        <f>_xll.qlRateHelperPillarDate($D75)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J75" s="18" t="e">
@@ -5577,7 +5577,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I76" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D76)</f>
+        <f>_xll.qlRateHelperPillarDate($D76)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J76" s="18" t="e">
@@ -5605,7 +5605,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I77" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D77)</f>
+        <f>_xll.qlRateHelperPillarDate($D77)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J77" s="18" t="e">
@@ -5633,7 +5633,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I78" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D78)</f>
+        <f>_xll.qlRateHelperPillarDate($D78)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J78" s="18" t="e">
@@ -5661,7 +5661,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I79" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D79)</f>
+        <f>_xll.qlRateHelperPillarDate($D79)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J79" s="18" t="e">
@@ -5689,7 +5689,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I80" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D80)</f>
+        <f>_xll.qlRateHelperPillarDate($D80)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J80" s="18" t="e">
@@ -5717,7 +5717,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I81" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D81)</f>
+        <f>_xll.qlRateHelperPillarDate($D81)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J81" s="18" t="e">
@@ -5745,7 +5745,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I82" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D82)</f>
+        <f>_xll.qlRateHelperPillarDate($D82)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J82" s="18" t="e">
@@ -5773,7 +5773,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I83" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D83)</f>
+        <f>_xll.qlRateHelperPillarDate($D83)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J83" s="18" t="e">
@@ -5801,7 +5801,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I84" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D84)</f>
+        <f>_xll.qlRateHelperPillarDate($D84)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J84" s="18" t="e">
@@ -5829,7 +5829,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I85" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D85)</f>
+        <f>_xll.qlRateHelperPillarDate($D85)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J85" s="18" t="e">
@@ -5857,7 +5857,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I86" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D86)</f>
+        <f>_xll.qlRateHelperPillarDate($D86)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J86" s="18" t="e">
@@ -5885,7 +5885,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I87" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D87)</f>
+        <f>_xll.qlRateHelperPillarDate($D87)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J87" s="18" t="e">
@@ -5913,7 +5913,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I88" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D88)</f>
+        <f>_xll.qlRateHelperPillarDate($D88)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J88" s="18" t="e">
@@ -5941,7 +5941,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I89" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D89)</f>
+        <f>_xll.qlRateHelperPillarDate($D89)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J89" s="18" t="e">
@@ -5969,7 +5969,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I90" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D90)</f>
+        <f>_xll.qlRateHelperPillarDate($D90)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J90" s="18" t="e">
@@ -5997,7 +5997,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I91" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D91)</f>
+        <f>_xll.qlRateHelperPillarDate($D91)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J91" s="18" t="e">
@@ -6025,7 +6025,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I92" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D92)</f>
+        <f>_xll.qlRateHelperPillarDate($D92)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J92" s="18" t="e">
@@ -6053,7 +6053,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I93" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D93)</f>
+        <f>_xll.qlRateHelperPillarDate($D93)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J93" s="18" t="e">
@@ -6081,7 +6081,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I94" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D94)</f>
+        <f>_xll.qlRateHelperPillarDate($D94)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J94" s="18" t="e">
@@ -6109,7 +6109,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I95" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D95)</f>
+        <f>_xll.qlRateHelperPillarDate($D95)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J95" s="18" t="e">
@@ -6137,7 +6137,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I96" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D96)</f>
+        <f>_xll.qlRateHelperPillarDate($D96)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J96" s="18" t="e">
@@ -6165,7 +6165,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I97" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D97)</f>
+        <f>_xll.qlRateHelperPillarDate($D97)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J97" s="18" t="e">
@@ -6193,7 +6193,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I98" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D98)</f>
+        <f>_xll.qlRateHelperPillarDate($D98)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J98" s="18" t="e">
@@ -6221,7 +6221,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I99" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D99)</f>
+        <f>_xll.qlRateHelperPillarDate($D99)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J99" s="18" t="e">
@@ -6249,7 +6249,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I100" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D100)</f>
+        <f>_xll.qlRateHelperPillarDate($D100)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J100" s="18" t="e">
@@ -6277,7 +6277,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I101" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D101)</f>
+        <f>_xll.qlRateHelperPillarDate($D101)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J101" s="18" t="e">
@@ -6305,7 +6305,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I102" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D102)</f>
+        <f>_xll.qlRateHelperPillarDate($D102)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J102" s="18" t="e">
@@ -6333,7 +6333,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I103" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D103)</f>
+        <f>_xll.qlRateHelperPillarDate($D103)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J103" s="18" t="e">
@@ -6361,7 +6361,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I104" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D104)</f>
+        <f>_xll.qlRateHelperPillarDate($D104)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J104" s="18" t="e">
@@ -6389,7 +6389,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I105" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D105)</f>
+        <f>_xll.qlRateHelperPillarDate($D105)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J105" s="18" t="e">
@@ -6417,7 +6417,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I106" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D106)</f>
+        <f>_xll.qlRateHelperPillarDate($D106)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J106" s="18" t="e">
@@ -6445,7 +6445,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I107" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D107)</f>
+        <f>_xll.qlRateHelperPillarDate($D107)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J107" s="18" t="e">
@@ -6473,7 +6473,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I108" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D108)</f>
+        <f>_xll.qlRateHelperPillarDate($D108)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J108" s="18" t="e">
@@ -6501,7 +6501,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I109" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D109)</f>
+        <f>_xll.qlRateHelperPillarDate($D109)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J109" s="18" t="e">
@@ -6529,7 +6529,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I110" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D110)</f>
+        <f>_xll.qlRateHelperPillarDate($D110)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J110" s="18" t="e">
@@ -6557,7 +6557,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I111" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D111)</f>
+        <f>_xll.qlRateHelperPillarDate($D111)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J111" s="18" t="e">
@@ -6585,7 +6585,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I112" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D112)</f>
+        <f>_xll.qlRateHelperPillarDate($D112)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J112" s="18" t="e">
@@ -6613,7 +6613,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I113" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D113)</f>
+        <f>_xll.qlRateHelperPillarDate($D113)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J113" s="18" t="e">
@@ -6641,7 +6641,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I114" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D114)</f>
+        <f>_xll.qlRateHelperPillarDate($D114)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J114" s="18" t="e">
@@ -6669,7 +6669,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I115" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D115)</f>
+        <f>_xll.qlRateHelperPillarDate($D115)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J115" s="18" t="e">
@@ -6697,7 +6697,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I116" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D116)</f>
+        <f>_xll.qlRateHelperPillarDate($D116)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J116" s="18" t="e">
@@ -6725,7 +6725,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I117" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D117)</f>
+        <f>_xll.qlRateHelperPillarDate($D117)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J117" s="18" t="e">
@@ -6753,7 +6753,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I118" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D118)</f>
+        <f>_xll.qlRateHelperPillarDate($D118)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J118" s="18" t="e">
@@ -6781,7 +6781,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I119" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D119)</f>
+        <f>_xll.qlRateHelperPillarDate($D119)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J119" s="18" t="e">
@@ -6809,7 +6809,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I120" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D120)</f>
+        <f>_xll.qlRateHelperPillarDate($D120)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J120" s="18" t="e">
@@ -6837,7 +6837,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I121" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D121)</f>
+        <f>_xll.qlRateHelperPillarDate($D121)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J121" s="18" t="e">
@@ -6865,7 +6865,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I122" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D122)</f>
+        <f>_xll.qlRateHelperPillarDate($D122)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J122" s="18" t="e">
@@ -6893,7 +6893,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I123" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D123)</f>
+        <f>_xll.qlRateHelperPillarDate($D123)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J123" s="18" t="e">
@@ -6921,7 +6921,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I124" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D124)</f>
+        <f>_xll.qlRateHelperPillarDate($D124)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J124" s="18" t="e">
@@ -6949,7 +6949,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I125" s="28" t="e">
-        <f>_xll.qlRateHelperLatestDate($D125)</f>
+        <f>_xll.qlRateHelperPillarDate($D125)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J125" s="18" t="e">
@@ -6977,7 +6977,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I126" s="30" t="e">
-        <f>_xll.qlRateHelperLatestDate($D126)</f>
+        <f>_xll.qlRateHelperPillarDate($D126)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J126" s="18" t="e">
@@ -7068,12 +7068,12 @@
         <v>HkdHiborON</v>
       </c>
       <c r="D3" s="38" t="str">
-        <f>Currency&amp;$B3&amp;"D"&amp;QuoteSuffix</f>
+        <f t="shared" ref="D3:D11" si="1">Currency&amp;$B3&amp;"D"&amp;QuoteSuffix</f>
         <v>HKDOND_Quote</v>
       </c>
       <c r="E3" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00138#0005</v>
+        <v>obj_00133#0001</v>
       </c>
       <c r="F3" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E3)</f>
@@ -7093,12 +7093,12 @@
         <v>HkdHiborSW</v>
       </c>
       <c r="D4" s="38" t="str">
-        <f>Currency&amp;$B4&amp;"D"&amp;QuoteSuffix</f>
+        <f t="shared" si="1"/>
         <v>HKDSWD_Quote</v>
       </c>
       <c r="E4" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013f#0003</v>
+        <v>obj_00135#0001</v>
       </c>
       <c r="F4" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E4)</f>
@@ -7118,12 +7118,12 @@
         <v>HkdHibor2W</v>
       </c>
       <c r="D5" s="38" t="str">
-        <f>Currency&amp;$B5&amp;"D"&amp;QuoteSuffix</f>
+        <f t="shared" si="1"/>
         <v>HKD2WD_Quote</v>
       </c>
       <c r="E5" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013e#0003</v>
+        <v>obj_00138#0001</v>
       </c>
       <c r="F5" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E5)</f>
@@ -7143,12 +7143,12 @@
         <v>HkdHibor1M</v>
       </c>
       <c r="D6" s="38" t="str">
-        <f>Currency&amp;$B6&amp;"D"&amp;QuoteSuffix</f>
+        <f t="shared" si="1"/>
         <v>HKD1MD_Quote</v>
       </c>
       <c r="E6" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00139#0003</v>
+        <v>obj_00139#0001</v>
       </c>
       <c r="F6" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -7168,12 +7168,12 @@
         <v>HkdHibor2M</v>
       </c>
       <c r="D7" s="38" t="str">
-        <f>Currency&amp;$B7&amp;"D"&amp;QuoteSuffix</f>
+        <f t="shared" si="1"/>
         <v>HKD2MD_Quote</v>
       </c>
       <c r="E7" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013d#0003</v>
+        <v>obj_00136#0001</v>
       </c>
       <c r="F7" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -7193,12 +7193,12 @@
         <v>HkdHibor3M</v>
       </c>
       <c r="D8" s="38" t="str">
-        <f>Currency&amp;$B8&amp;"D"&amp;QuoteSuffix</f>
+        <f t="shared" si="1"/>
         <v>HKD3MD_Quote</v>
       </c>
       <c r="E8" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013a#0003</v>
+        <v>obj_0013b#0001</v>
       </c>
       <c r="F8" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -7218,12 +7218,12 @@
         <v>HkdHibor6M</v>
       </c>
       <c r="D9" s="38" t="str">
-        <f>Currency&amp;$B9&amp;"D"&amp;QuoteSuffix</f>
+        <f t="shared" si="1"/>
         <v>HKD6MD_Quote</v>
       </c>
       <c r="E9" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00140#0003</v>
+        <v>obj_0013a#0001</v>
       </c>
       <c r="F9" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -7243,12 +7243,12 @@
         <v>HkdHibor9M</v>
       </c>
       <c r="D10" s="38" t="str">
-        <f>Currency&amp;$B10&amp;"D"&amp;QuoteSuffix</f>
+        <f t="shared" si="1"/>
         <v>HKD9MD_Quote</v>
       </c>
       <c r="E10" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013c#0003</v>
+        <v>obj_00134#0001</v>
       </c>
       <c r="F10" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -7268,12 +7268,12 @@
         <v>HkdHibor1Y</v>
       </c>
       <c r="D11" s="38" t="str">
-        <f>Currency&amp;$B11&amp;"D"&amp;QuoteSuffix</f>
+        <f t="shared" si="1"/>
         <v>HKD1YD_Quote</v>
       </c>
       <c r="E11" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013b#0003</v>
+        <v>obj_00137#0001</v>
       </c>
       <c r="F11" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -7308,7 +7308,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="L6" sqref="L6:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -7441,7 +7441,7 @@
       <c r="K4" s="48"/>
       <c r="L4" s="63" t="str">
         <f>_xll.qlIborIndex(,FamilyName,J2,P4,Currency,Q4,R4,S4,T4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00120#0001</v>
+        <v>obj_0011b#0001</v>
       </c>
       <c r="M4" s="64" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -7519,8 +7519,8 @@
         <v>HKDQM3H1Y_Quote</v>
       </c>
       <c r="L6" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K6,$B6,$D6,Calendar,$G6,$H6,$I6,$L$4,$J6,C6&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00127#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K6,$B6,$D6,Calendar,$G6,$H6,$I6,$L$4,$J6,C6&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00124#0001</v>
       </c>
       <c r="M6" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -7565,8 +7565,8 @@
         <v>HKDQM3H15M_Quote</v>
       </c>
       <c r="L7" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K7,$B7,$D7,Calendar,$G7,$H7,$I7,$L$4,$J7,C7&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00130#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K7,$B7,$D7,Calendar,$G7,$H7,$I7,$L$4,$J7,C7&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00122#0001</v>
       </c>
       <c r="M7" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -7611,8 +7611,8 @@
         <v>HKDQM3H18M_Quote</v>
       </c>
       <c r="L8" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K8,$B8,$D8,Calendar,$G8,$H8,$I8,$L$4,$J8,C8&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00128#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K8,$B8,$D8,Calendar,$G8,$H8,$I8,$L$4,$J8,C8&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00125#0001</v>
       </c>
       <c r="M8" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -7657,7 +7657,7 @@
         <v>HKDQM3H21M_Quote</v>
       </c>
       <c r="L9" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K9,$B9,$D9,Calendar,$G9,$H9,$I9,$L$4,$J9,C9&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(,$K9,$B9,$D9,Calendar,$G9,$H9,$I9,$L$4,$J9,C9&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
         <v>obj_0012c#0001</v>
       </c>
       <c r="M9" s="61" t="str">
@@ -7703,8 +7703,8 @@
         <v>HKDQM3H2Y_Quote</v>
       </c>
       <c r="L10" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K10,$B10,$D10,Calendar,$G10,$H10,$I10,$L$4,$J10,C10&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00136#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K10,$B10,$D10,Calendar,$G10,$H10,$I10,$L$4,$J10,C10&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00131#0001</v>
       </c>
       <c r="M10" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -7749,8 +7749,8 @@
         <v>HKDQM3H3Y_Quote</v>
       </c>
       <c r="L11" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K11,$B11,$D11,Calendar,$G11,$H11,$I11,$L$4,$J11,C11&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00134#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K11,$B11,$D11,Calendar,$G11,$H11,$I11,$L$4,$J11,C11&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00129#0001</v>
       </c>
       <c r="M11" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -7795,8 +7795,8 @@
         <v>HKDQM3H4Y_Quote</v>
       </c>
       <c r="L12" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K12,$B12,$D12,Calendar,$G12,$H12,$I12,$L$4,$J12,C12&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00131#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K12,$B12,$D12,Calendar,$G12,$H12,$I12,$L$4,$J12,C12&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0012e#0001</v>
       </c>
       <c r="M12" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -7841,8 +7841,8 @@
         <v>HKDQM3H5Y_Quote</v>
       </c>
       <c r="L13" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K13,$B13,$D13,Calendar,$G13,$H13,$I13,$L$4,$J13,C13&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00123#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K13,$B13,$D13,Calendar,$G13,$H13,$I13,$L$4,$J13,C13&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00127#0001</v>
       </c>
       <c r="M13" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -7887,8 +7887,8 @@
         <v>HKDQM3H6Y_Quote</v>
       </c>
       <c r="L14" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K14,$B14,$D14,Calendar,$G14,$H14,$I14,$L$4,$J14,C14&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00125#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K14,$B14,$D14,Calendar,$G14,$H14,$I14,$L$4,$J14,C14&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0011f#0001</v>
       </c>
       <c r="M14" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -7933,8 +7933,8 @@
         <v>HKDQM3H7Y_Quote</v>
       </c>
       <c r="L15" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K15,$B15,$D15,Calendar,$G15,$H15,$I15,$L$4,$J15,C15&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00137#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K15,$B15,$D15,Calendar,$G15,$H15,$I15,$L$4,$J15,C15&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00132#0001</v>
       </c>
       <c r="M15" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -7979,8 +7979,8 @@
         <v>HKDQM3H8Y_Quote</v>
       </c>
       <c r="L16" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K16,$B16,$D16,Calendar,$G16,$H16,$I16,$L$4,$J16,C16&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012a#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K16,$B16,$D16,Calendar,$G16,$H16,$I16,$L$4,$J16,C16&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00128#0001</v>
       </c>
       <c r="M16" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -8025,8 +8025,8 @@
         <v>HKDQM3H9Y_Quote</v>
       </c>
       <c r="L17" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K17,$B17,$D17,Calendar,$G17,$H17,$I17,$L$4,$J17,C17&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012d#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K17,$B17,$D17,Calendar,$G17,$H17,$I17,$L$4,$J17,C17&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00121#0001</v>
       </c>
       <c r="M17" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -8071,8 +8071,8 @@
         <v>HKDQM3H10Y_Quote</v>
       </c>
       <c r="L18" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K18,$B18,$D18,Calendar,$G18,$H18,$I18,$L$4,$J18,C18&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00122#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K18,$B18,$D18,Calendar,$G18,$H18,$I18,$L$4,$J18,C18&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0011d#0001</v>
       </c>
       <c r="M18" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -8117,8 +8117,8 @@
         <v>HKDQM3H11Y_Quote</v>
       </c>
       <c r="L19" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K19,$B19,$D19,Calendar,$G19,$H19,$I19,$L$4,$J19,C19&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00133#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K19,$B19,$D19,Calendar,$G19,$H19,$I19,$L$4,$J19,C19&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0012b#0001</v>
       </c>
       <c r="M19" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -8163,8 +8163,8 @@
         <v>HKDQM3H12Y_Quote</v>
       </c>
       <c r="L20" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K20,$B20,$D20,Calendar,$G20,$H20,$I20,$L$4,$J20,C20&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012e#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K20,$B20,$D20,Calendar,$G20,$H20,$I20,$L$4,$J20,C20&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00123#0001</v>
       </c>
       <c r="M20" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -8209,8 +8209,8 @@
         <v>HKDQM3H13Y_Quote</v>
       </c>
       <c r="L21" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K21,$B21,$D21,Calendar,$G21,$H21,$I21,$L$4,$J21,C21&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00124#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K21,$B21,$D21,Calendar,$G21,$H21,$I21,$L$4,$J21,C21&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0012a#0001</v>
       </c>
       <c r="M21" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -8255,8 +8255,8 @@
         <v>HKDQM3H14Y_Quote</v>
       </c>
       <c r="L22" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K22,$B22,$D22,Calendar,$G22,$H22,$I22,$L$4,$J22,C22&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012f#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K22,$B22,$D22,Calendar,$G22,$H22,$I22,$L$4,$J22,C22&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0012d#0001</v>
       </c>
       <c r="M22" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -8301,8 +8301,8 @@
         <v>HKDQM3H15Y_Quote</v>
       </c>
       <c r="L23" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K23,$B23,$D23,Calendar,$G23,$H23,$I23,$L$4,$J23,C23&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00121#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K23,$B23,$D23,Calendar,$G23,$H23,$I23,$L$4,$J23,C23&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0011c#0001</v>
       </c>
       <c r="M23" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -8347,8 +8347,8 @@
         <v>HKDQM3H16Y_Quote</v>
       </c>
       <c r="L24" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K24,$B24,$D24,Calendar,$G24,$H24,$I24,$L$4,$J24,C24&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012b#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K24,$B24,$D24,Calendar,$G24,$H24,$I24,$L$4,$J24,C24&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0011e#0001</v>
       </c>
       <c r="M24" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -8393,8 +8393,8 @@
         <v>HKDQM3H17Y_Quote</v>
       </c>
       <c r="L25" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K25,$B25,$D25,Calendar,$G25,$H25,$I25,$L$4,$J25,C25&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00126#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K25,$B25,$D25,Calendar,$G25,$H25,$I25,$L$4,$J25,C25&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0012f#0001</v>
       </c>
       <c r="M25" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -8439,8 +8439,8 @@
         <v>HKDQM3H18Y_Quote</v>
       </c>
       <c r="L26" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K26,$B26,$D26,Calendar,$G26,$H26,$I26,$L$4,$J26,C26&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00129#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K26,$B26,$D26,Calendar,$G26,$H26,$I26,$L$4,$J26,C26&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00126#0001</v>
       </c>
       <c r="M26" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -8485,8 +8485,8 @@
         <v>HKDQM3H19Y_Quote</v>
       </c>
       <c r="L27" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K27,$B27,$D27,Calendar,$G27,$H27,$I27,$L$4,$J27,C27&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00132#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K27,$B27,$D27,Calendar,$G27,$H27,$I27,$L$4,$J27,C27&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00120#0001</v>
       </c>
       <c r="M27" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -8531,8 +8531,8 @@
         <v>HKDQM3H20Y_Quote</v>
       </c>
       <c r="L28" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$K28,$B28,$D28,Calendar,$G28,$H28,$I28,$L$4,$J28,C28&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00135#0001</v>
+        <f>_xll.qlSwapRateHelper2(,$K28,$B28,$D28,Calendar,$G28,$H28,$I28,$L$4,$J28,C28&amp;"D",Discounting2,,,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00130#0001</v>
       </c>
       <c r="M28" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>

</xml_diff>